<commit_message>
July 29 candidate update
</commit_message>
<xml_diff>
--- a/data/dcboe/excel-clean/dcboe-ballot-2024-07-24.xlsx
+++ b/data/dcboe/excel-clean/dcboe-ballot-2024-07-24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devin/Projects/openanc/data/dcboe/excel-clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFF4BA9-73FD-5248-8109-F45C2049D777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D6CDB0-6647-9142-94B8-8CB26AAAE3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{756E3DF6-12F0-7E42-BCA7-694482500748}"/>
   </bookViews>
@@ -2384,7 +2384,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>